<commit_message>
add HkmcFcaAdap's arxml for R2
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcVehOutputAdap/VehOutputAdap_SignalMatrix_V3_R2.xlsx
+++ b/R2/02_SignalMatrix/HkmcVehOutputAdap/VehOutputAdap_SignalMatrix_V3_R2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R2\02_SignalMatrix\HkmcVehOutputAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E9A6D3-93CE-47CE-9B3E-262BE53D441B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5972FD45-E71F-462A-B674-60674699F335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
@@ -12322,7 +12322,7 @@
   <dimension ref="A1:K556"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G154" sqref="G154"/>
+      <selection activeCell="G156" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>

</xml_diff>